<commit_message>
corrected name in 759, corrected columns in 1476, corrected 0 in 2002
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_2002.xlsx
+++ b/fastqFiles/fastq_2002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1F1338-988F-BC4D-A5EA-741DEB17AB18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3769F80-449C-AF40-89DA-4509743C3A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="57">
   <si>
     <t>libraryDate</t>
   </si>
@@ -40,12 +40,6 @@
     <t>fastqFileName</t>
   </si>
   <si>
-    <t>2.10.17</t>
-  </si>
-  <si>
-    <t>2.1.17</t>
-  </si>
-  <si>
     <t>sequence/run_2002_samples/2002_Brent_A_TGAGGTT_S2_R1_001.fastq.gz</t>
   </si>
   <si>
@@ -194,6 +188,9 @@
   </si>
   <si>
     <t>H.BROWN</t>
+  </si>
+  <si>
+    <t>02.10.17</t>
   </si>
 </sst>
 </file>
@@ -597,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50:G58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -625,10 +622,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -637,18 +634,18 @@
         <v>2002</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -657,18 +654,18 @@
         <v>2002</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -677,18 +674,18 @@
         <v>2002</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -697,18 +694,18 @@
         <v>2002</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -717,18 +714,18 @@
         <v>2002</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -737,18 +734,18 @@
         <v>2002</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -757,18 +754,18 @@
         <v>2002</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -777,18 +774,18 @@
         <v>2002</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -797,18 +794,18 @@
         <v>2002</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -817,18 +814,18 @@
         <v>2002</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -837,18 +834,18 @@
         <v>2002</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -857,18 +854,18 @@
         <v>2002</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -877,18 +874,18 @@
         <v>2002</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -897,18 +894,18 @@
         <v>2002</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -917,18 +914,18 @@
         <v>2002</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -937,18 +934,18 @@
         <v>2002</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -957,18 +954,18 @@
         <v>2002</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -977,18 +974,18 @@
         <v>2002</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -997,18 +994,18 @@
         <v>2002</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1017,18 +1014,18 @@
         <v>2002</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1037,18 +1034,18 @@
         <v>2002</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1057,18 +1054,18 @@
         <v>2002</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1077,18 +1074,18 @@
         <v>2002</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1097,18 +1094,18 @@
         <v>2002</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1117,18 +1114,18 @@
         <v>2002</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1137,18 +1134,18 @@
         <v>2002</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1157,18 +1154,18 @@
         <v>2002</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -1177,18 +1174,18 @@
         <v>2002</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1197,18 +1194,18 @@
         <v>2002</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -1217,18 +1214,18 @@
         <v>2002</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -1237,18 +1234,18 @@
         <v>2002</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -1257,18 +1254,18 @@
         <v>2002</v>
       </c>
       <c r="E33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C34">
         <v>33</v>
@@ -1277,18 +1274,18 @@
         <v>2002</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -1297,18 +1294,18 @@
         <v>2002</v>
       </c>
       <c r="E35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -1317,18 +1314,18 @@
         <v>2002</v>
       </c>
       <c r="E36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -1337,18 +1334,18 @@
         <v>2002</v>
       </c>
       <c r="E37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C38">
         <v>37</v>
@@ -1357,18 +1354,18 @@
         <v>2002</v>
       </c>
       <c r="E38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -1377,18 +1374,18 @@
         <v>2002</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -1397,18 +1394,18 @@
         <v>2002</v>
       </c>
       <c r="E40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -1417,18 +1414,18 @@
         <v>2002</v>
       </c>
       <c r="E41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -1437,18 +1434,18 @@
         <v>2002</v>
       </c>
       <c r="E42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -1457,18 +1454,18 @@
         <v>2002</v>
       </c>
       <c r="E43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -1477,18 +1474,18 @@
         <v>2002</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -1497,18 +1494,18 @@
         <v>2002</v>
       </c>
       <c r="E45" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46">
         <v>45</v>
@@ -1517,18 +1514,18 @@
         <v>2002</v>
       </c>
       <c r="E46" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F46" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C47">
         <v>46</v>
@@ -1537,18 +1534,18 @@
         <v>2002</v>
       </c>
       <c r="E47" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F47" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -1557,18 +1554,18 @@
         <v>2002</v>
       </c>
       <c r="E48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C49">
         <v>48</v>
@@ -1577,10 +1574,10 @@
         <v>2002</v>
       </c>
       <c r="E49" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>